<commit_message>
Pdfs y nuevo excel
</commit_message>
<xml_diff>
--- a/clean_data/model_IG.xlsx
+++ b/clean_data/model_IG.xlsx
@@ -442,17 +442,17 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -462,32 +462,32 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -497,12 +497,12 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -512,7 +512,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -527,62 +527,62 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
@@ -602,7 +602,7 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
@@ -617,7 +617,7 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
@@ -627,42 +627,42 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
@@ -672,7 +672,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -682,17 +682,17 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
@@ -702,12 +702,12 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
@@ -717,17 +717,17 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60">
@@ -747,7 +747,7 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64">
@@ -757,12 +757,12 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
@@ -772,32 +772,32 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74">
@@ -817,12 +817,12 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79">
@@ -832,7 +832,7 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81">
@@ -842,12 +842,12 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84">
@@ -862,22 +862,22 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90">
@@ -887,7 +887,7 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92">
@@ -897,32 +897,32 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99">
@@ -932,7 +932,7 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101">
@@ -947,37 +947,37 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110">
@@ -987,12 +987,12 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113">
@@ -1002,22 +1002,22 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118">
@@ -1027,7 +1027,7 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120">
@@ -1037,22 +1037,22 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125">
@@ -1062,17 +1062,17 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129">
@@ -1097,22 +1097,22 @@
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137">
@@ -1127,52 +1127,52 @@
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149">
@@ -1187,7 +1187,7 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152">
@@ -1202,37 +1202,37 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161">
@@ -1242,7 +1242,7 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="163">
@@ -1257,7 +1257,7 @@
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166">
@@ -1272,22 +1272,22 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="172">
@@ -1297,7 +1297,7 @@
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174">
@@ -1312,12 +1312,12 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178">
@@ -1342,47 +1342,47 @@
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="191">
@@ -1392,27 +1392,27 @@
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="197">
@@ -1422,27 +1422,27 @@
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="203">
@@ -1452,52 +1452,52 @@
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="214">
@@ -1512,7 +1512,7 @@
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="217">
@@ -1527,12 +1527,12 @@
     </row>
     <row r="219">
       <c r="A219" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="221">
@@ -1542,7 +1542,7 @@
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="223">
@@ -1557,32 +1557,32 @@
     </row>
     <row r="225">
       <c r="A225" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="231">
@@ -1592,7 +1592,7 @@
     </row>
     <row r="232">
       <c r="A232" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="233">
@@ -1602,12 +1602,12 @@
     </row>
     <row r="234">
       <c r="A234" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="236">
@@ -1617,37 +1617,37 @@
     </row>
     <row r="237">
       <c r="A237" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="244">
@@ -1657,17 +1657,17 @@
     </row>
     <row r="245">
       <c r="A245" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="248">
@@ -1677,7 +1677,7 @@
     </row>
     <row r="249">
       <c r="A249" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="250">
@@ -1687,12 +1687,12 @@
     </row>
     <row r="251">
       <c r="A251" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="253">
@@ -1712,62 +1712,62 @@
     </row>
     <row r="256">
       <c r="A256" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>